<commit_message>
BIS-1630: Fixed core-plugins tests
</commit_message>
<xml_diff>
--- a/core-plugin-openbis/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/xls/with_blanks.xlsx
+++ b/core-plugin-openbis/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/xls/with_blanks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TYPES" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="98">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -323,10 +323,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -455,7 +454,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,10 +481,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -547,11 +542,11 @@
   </sheetPr>
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
@@ -1173,9 +1168,8 @@
       <c r="B32" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="7" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C32" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>17</v>
@@ -1189,7 +1183,7 @@
       <c r="G32" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J32" s="0" t="s">
@@ -1259,13 +1253,13 @@
       <c r="A42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="G42" s="8"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="G43" s="8"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
@@ -1394,11 +1388,11 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
   </cols>
@@ -1410,7 +1404,7 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1438,7 +1432,7 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1480,8 +1474,8 @@
       <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1491,13 +1485,13 @@
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1561,22 +1555,22 @@
       <c r="A23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1597,31 +1591,31 @@
       <c r="H25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="12" t="s">
         <v>31</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="O25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="P25" s="15" t="s">
+      <c r="P25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="Q25" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1640,7 +1634,7 @@
         <v>17</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="15" t="s">
         <v>91</v>
       </c>
       <c r="I26" s="0" t="s">
@@ -1672,7 +1666,7 @@
       <c r="F27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="16" t="s">
         <v>96</v>
       </c>
       <c r="I27" s="0" t="s">
@@ -1692,7 +1686,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1727,18 +1721,18 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="15"/>
       <c r="L29" s="6"/>
       <c r="P29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="16"/>
       <c r="J30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>

</xml_diff>